<commit_message>
Experimenting with Unity DOTS Physics for Detection AI raycasts
</commit_message>
<xml_diff>
--- a/Assets/Scripts/IAUS/Curves.xlsx
+++ b/Assets/Scripts/IAUS/Curves.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Main Game Folder\ECS IAUS sytstem\Assets\Scripts\IAUS\ECS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Main Game Folder\ECS IAUS sytstem\Assets\Scripts\IAUS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -197,37 +197,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.99929352122393278</c:v>
+                  <c:v>-3.427916099383399E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.99770062259718262</c:v>
+                  <c:v>-4.9666306624440715E-4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.99254772766787358</c:v>
+                  <c:v>9.5173773371015513E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.97617181149515997</c:v>
+                  <c:v>0.30640798364644595</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.92693155525451087</c:v>
+                  <c:v>0.5935920163535543</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.80050775077933256</c:v>
+                  <c:v>0.80482622662898451</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.57499999999999996</c:v>
+                  <c:v>0.90049666306624443</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.34949224922066746</c:v>
+                  <c:v>0.9342791609938339</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.2230684447454892</c:v>
+                  <c:v>0.94512573721099469</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.17382818850483997</c:v>
+                  <c:v>0.94850013331132521</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.15745227233212639</c:v>
+                  <c:v>0.9495395546737434</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -420,11 +420,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-114968928"/>
-        <c:axId val="-114969472"/>
+        <c:axId val="-882779408"/>
+        <c:axId val="-882791376"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-114968928"/>
+        <c:axId val="-882779408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -467,7 +467,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-114969472"/>
+        <c:crossAx val="-882791376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -475,7 +475,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-114969472"/>
+        <c:axId val="-882791376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -526,7 +526,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-114968928"/>
+        <c:crossAx val="-882779408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1461,10 +1461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F22"/>
+  <dimension ref="A2:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12:F22"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1495,7 +1495,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>0.85</v>
+        <v>-1</v>
       </c>
       <c r="D3">
         <v>-0.85</v>
@@ -1512,7 +1512,7 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>0.15</v>
+        <v>0.95</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -1529,7 +1529,7 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>0.6</v>
+        <v>0.35</v>
       </c>
       <c r="D5">
         <v>0.6</v>
@@ -1575,10 +1575,10 @@
       </c>
       <c r="C12">
         <f>C$3*1/(1+POWER((1000*C$2*EXP(1)),($B12-C$5)))+C$4</f>
-        <v>0.99929352122393278</v>
+        <v>-3.427916099383399E-2</v>
       </c>
       <c r="D12">
-        <f t="shared" ref="D12:F22" si="0">D$3*1/(1+POWER((1000*D$2*EXP(1)),($B12-D$5)))+D$4</f>
+        <f t="shared" ref="D12:F27" si="0">D$3*1/(1+POWER((1000*D$2*EXP(1)),($B12-D$5)))+D$4</f>
         <v>0.15080759462076365</v>
       </c>
       <c r="E12">
@@ -1600,8 +1600,8 @@
         <v>0.1</v>
       </c>
       <c r="C13">
-        <f t="shared" ref="C13:C22" si="1">C$3*1/(1+POWER((1000*C$2*EXP(1)),($B13-C$5)))+C$4</f>
-        <v>0.99770062259718262</v>
+        <f t="shared" ref="C13:F28" si="1">C$3*1/(1+POWER((1000*C$2*EXP(1)),($B13-C$5)))+C$4</f>
+        <v>-4.9666306624440715E-4</v>
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
@@ -1627,7 +1627,7 @@
       </c>
       <c r="C14">
         <f t="shared" si="1"/>
-        <v>0.99254772766787358</v>
+        <v>9.5173773371015513E-2</v>
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
@@ -1653,7 +1653,7 @@
       </c>
       <c r="C15">
         <f t="shared" si="1"/>
-        <v>0.97617181149515997</v>
+        <v>0.30640798364644595</v>
       </c>
       <c r="D15">
         <f t="shared" si="0"/>
@@ -1679,7 +1679,7 @@
       </c>
       <c r="C16">
         <f t="shared" si="1"/>
-        <v>0.92693155525451087</v>
+        <v>0.5935920163535543</v>
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
@@ -1705,7 +1705,7 @@
       </c>
       <c r="C17">
         <f t="shared" si="1"/>
-        <v>0.80050775077933256</v>
+        <v>0.80482622662898451</v>
       </c>
       <c r="D17">
         <f t="shared" si="0"/>
@@ -1731,7 +1731,7 @@
       </c>
       <c r="C18">
         <f t="shared" si="1"/>
-        <v>0.57499999999999996</v>
+        <v>0.90049666306624443</v>
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
@@ -1757,7 +1757,7 @@
       </c>
       <c r="C19">
         <f t="shared" si="1"/>
-        <v>0.34949224922066746</v>
+        <v>0.9342791609938339</v>
       </c>
       <c r="D19">
         <f t="shared" si="0"/>
@@ -1783,7 +1783,7 @@
       </c>
       <c r="C20">
         <f t="shared" si="1"/>
-        <v>0.2230684447454892</v>
+        <v>0.94512573721099469</v>
       </c>
       <c r="D20">
         <f t="shared" si="0"/>
@@ -1809,7 +1809,7 @@
       </c>
       <c r="C21">
         <f t="shared" si="1"/>
-        <v>0.17382818850483997</v>
+        <v>0.94850013331132521</v>
       </c>
       <c r="D21">
         <f t="shared" si="0"/>
@@ -1835,7 +1835,7 @@
       </c>
       <c r="C22">
         <f t="shared" si="1"/>
-        <v>0.15745227233212639</v>
+        <v>0.9495395546737434</v>
       </c>
       <c r="D22">
         <f t="shared" si="0"/>
@@ -1848,6 +1848,188 @@
       <c r="F22">
         <f t="shared" si="0"/>
         <v>0.99051770092623315</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <f t="shared" ref="A23:B23" si="3">A22+0.1</f>
+        <v>1.0999999999999999</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="3"/>
+        <v>1.0999999999999999</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="1"/>
+        <v>0.949858749404763</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>0.99743003849844614</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>5.2299377402817482E-2</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="0"/>
+        <v>0.99700675072171963</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <f t="shared" ref="A24:B24" si="4">A23+0.1</f>
+        <v>1.2</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="4"/>
+        <v>1.2</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="1"/>
+        <v>0.94995667821208785</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>0.99919240537923626</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="0"/>
+        <v>5.0706478776067279E-2</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="0"/>
+        <v>0.99905938979463993</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <f t="shared" ref="A25:B25" si="5">A24+0.1</f>
+        <v>1.3</v>
+      </c>
+      <c r="B25">
+        <f t="shared" si="5"/>
+        <v>1.3</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="1"/>
+        <v>0.94998671403916057</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="0"/>
+        <v>0.99974657976228698</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>5.021678189573632E-2</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="0"/>
+        <v>0.9997048399584284</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <f t="shared" ref="A26:B26" si="6">A25+0.1</f>
+        <v>1.4000000000000001</v>
+      </c>
+      <c r="B26">
+        <f t="shared" si="6"/>
+        <v>1.4000000000000001</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="1"/>
+        <v>0.94999592553567169</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="0"/>
+        <v>0.99992051325137576</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="0"/>
+        <v>5.0066492607181691E-2</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="0"/>
+        <v>0.99990742131630828</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <f t="shared" ref="A27:B27" si="7">A26+0.1</f>
+        <v>1.5000000000000002</v>
+      </c>
+      <c r="B27">
+        <f t="shared" si="7"/>
+        <v>1.5000000000000002</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="1"/>
+        <v>0.94999875047399751</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="0"/>
+        <v>0.99997507201566671</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="0"/>
+        <v>5.0020392499894789E-2</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="0"/>
+        <v>0.9999709662300118</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <f t="shared" ref="A28:B28" si="8">A27+0.1</f>
+        <v>1.6000000000000003</v>
+      </c>
+      <c r="B28">
+        <f t="shared" si="8"/>
+        <v>1.6000000000000003</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="1"/>
+        <v>0.94999961680553635</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="1"/>
+        <v>0.99999218263377132</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="1"/>
+        <v>5.0006253904486257E-2</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="1"/>
+        <v>0.999990895067569</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <f t="shared" ref="A29:B29" si="9">A28+0.1</f>
+        <v>1.7000000000000004</v>
+      </c>
+      <c r="B29">
+        <f t="shared" si="9"/>
+        <v>1.7000000000000004</v>
+      </c>
+      <c r="C29">
+        <f t="shared" ref="C29:F29" si="10">C$3*1/(1+POWER((1000*C$2*EXP(1)),($B29-C$5)))+C$4</f>
+        <v>0.94999988248511158</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="10"/>
+        <v>0.99999754852339739</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="10"/>
+        <v>5.0001917904644769E-2</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="10"/>
+        <v>0.9999971447507805</v>
       </c>
     </row>
   </sheetData>

</xml_diff>